<commit_message>
Se agregaron unos errores
</commit_message>
<xml_diff>
--- a/Calculo de primeros y siguientes.xlsx
+++ b/Calculo de primeros y siguientes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Camran1234\source\repos\Proyecto2_Lenguajes_Analizador_Sintactico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{53614E08-193E-463F-94C4-1AB0D12A5614}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C4CD29-F0A9-43B6-A0EB-419F63589245}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{02987567-9D64-471F-979D-34ECD3E91EEB}"/>
+    <workbookView xWindow="10200" yWindow="2208" windowWidth="17280" windowHeight="8964" xr2:uid="{02987567-9D64-471F-979D-34ECD3E91EEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Primeros" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="85">
   <si>
     <t>Calculo de primeros</t>
   </si>
@@ -165,9 +165,6 @@
     <t>)</t>
   </si>
   <si>
-    <t>Entero, Cadena, Chart, Decimal, True, False</t>
-  </si>
-  <si>
     <t>SI</t>
   </si>
   <si>
@@ -198,9 +195,6 @@
     <t>Variable, entero, decimal, cadena chart, true, false</t>
   </si>
   <si>
-    <t>+, ;</t>
-  </si>
-  <si>
     <t>SINO_SI, SINO, e</t>
   </si>
   <si>
@@ -225,18 +219,12 @@
     <t>$</t>
   </si>
   <si>
-    <t>Pendiente</t>
-  </si>
-  <si>
     <t>P</t>
   </si>
   <si>
     <t>K'</t>
   </si>
   <si>
-    <t>"," , ;</t>
-  </si>
-  <si>
     <t>= , " , "</t>
   </si>
   <si>
@@ -258,21 +246,12 @@
     <t>Entero, Cadena, Chart, Decimal, Boolean, }, SI, MIENTRAS, HACER, DESDE, IMPRIMIR, Leer</t>
   </si>
   <si>
-    <t>Entero, Cadena, Chart, Decimal, Boolean, }, SI, MIENTRAS, HACER, DESDE, ; IMPRIMIR, Leer</t>
-  </si>
-  <si>
     <t>Entero, Cadena, Chart, Decimal, Boolean, }, SI, MIENTRAS, HACER, DESDE, IMPRIMIR, Leer, , }</t>
   </si>
   <si>
-    <t>Entero, Cadena, Chart, Decimal, Boolean, }, SI, MIENTRAS, HACER, DESDE, IMPRIMIR, Leer, }</t>
-  </si>
-  <si>
     <t>$, SINO_SI, SINO, e, Entero, Cadena, Chart, Decimal, Boolean, }, SI, MIENTRAS, HACER, DESDE, IMPRIMIR, Leer</t>
   </si>
   <si>
-    <t>&gt;, &gt;=, &lt;, &lt;=, !, == , Variable, entero, decimal, cadena chart, true, false, &amp;&amp;, ||, ), {, +, INCREMENTO, HASTA</t>
-  </si>
-  <si>
     <t>Entero, Cadena, Chart, Decimal, Boolean, SI, MIENTRAS, }, HACER, DESDE, SINO_SI, SINO, e IMPRIMIR, Leer, ;, {</t>
   </si>
   <si>
@@ -280,6 +259,27 @@
   </si>
   <si>
     <t>Variable, entero, decimal, cadena chart, true, false, ), {</t>
+  </si>
+  <si>
+    <t>Primeros</t>
+  </si>
+  <si>
+    <t>Entero, Cadena, Chart, Decimal, Boolean</t>
+  </si>
+  <si>
+    <t>"," , e</t>
+  </si>
+  <si>
+    <t>+, e</t>
+  </si>
+  <si>
+    <t>&gt;, &gt;=, &lt;, &lt;=, !, == , Variable, entero, decimal, cadena chart, true, false, &amp;&amp;, ||, ), {, +, INCREMENTO, HASTA, ;</t>
+  </si>
+  <si>
+    <t>Entero, Cadena, Chart, Decimal, Boolean, }, SI, MIENTRAS, HACER, DESDE IMPRIMIR, Leer</t>
+  </si>
+  <si>
+    <t>{, ;</t>
   </si>
 </sst>
 </file>
@@ -323,7 +323,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -346,17 +346,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -372,7 +361,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -689,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F48AB1A-0610-42A2-9EC7-30248C957360}">
-  <dimension ref="B3:G50"/>
+  <dimension ref="B3:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -702,29 +691,29 @@
     <col min="6" max="6" width="93.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="E3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F3" t="s">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1</v>
+        <v>78</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
@@ -735,10 +724,10 @@
         <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
@@ -749,13 +738,10 @@
         <v>4</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
@@ -766,10 +752,10 @@
         <v>5</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
@@ -780,24 +766,24 @@
         <v>6</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
@@ -808,10 +794,10 @@
         <v>8</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
@@ -822,29 +808,29 @@
         <v>9</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>39</v>
@@ -853,124 +839,124 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>51</v>
+        <v>18</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>70</v>
+        <v>19</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>55</v>
+        <v>20</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
-        <v>68</v>
+        <v>10</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>22</v>
@@ -981,49 +967,49 @@
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>57</v>
+        <v>22</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>47</v>
@@ -1032,29 +1018,29 @@
         <v>25</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B28" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>26</v>
@@ -1065,24 +1051,24 @@
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B29" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>27</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B30" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>28</v>
@@ -1093,52 +1079,52 @@
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B31" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>29</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B32" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B33" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B34" s="2" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>31</v>
@@ -1149,153 +1135,153 @@
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B35" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B36" s="2" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>32</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B37" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B38" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B39" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B40" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>36</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B41" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B42" s="2" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B43" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>38</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B44" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B45" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>51</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>45</v>
@@ -1303,47 +1289,23 @@
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B46" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>62</v>
+        <v>67</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B47" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B48" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B49" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B50" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C50" s="2" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Correccion Errores Gramaticas, Finales
</commit_message>
<xml_diff>
--- a/Calculo de primeros y siguientes.xlsx
+++ b/Calculo de primeros y siguientes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Camran1234\source\repos\Proyecto2_Lenguajes_Analizador_Sintactico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C4CD29-F0A9-43B6-A0EB-419F63589245}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AD8087-CB4D-443D-9C54-24711FBFDBA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10200" yWindow="2208" windowWidth="17280" windowHeight="8964" xr2:uid="{02987567-9D64-471F-979D-34ECD3E91EEB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{02987567-9D64-471F-979D-34ECD3E91EEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Primeros" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="88">
   <si>
     <t>Calculo de primeros</t>
   </si>
@@ -234,9 +234,6 @@
     <t>Variable, entero, decimal, cadena chart, true, false, INCREMENTO</t>
   </si>
   <si>
-    <t>= , " , " , ; , +, )</t>
-  </si>
-  <si>
     <t>Entero, Cadena, Chart, Decimal, Boolean, SI, }, MIENTRAS, HACER, DESDE, IMPRIMIR, Leer</t>
   </si>
   <si>
@@ -280,6 +277,18 @@
   </si>
   <si>
     <t>{, ;</t>
+  </si>
+  <si>
+    <t>_W</t>
+  </si>
+  <si>
+    <t>!</t>
+  </si>
+  <si>
+    <t>Variable, entero, decimal, cadena chart, true, false, !</t>
+  </si>
+  <si>
+    <t>= , " , " , ; , +, ), &amp;&amp;, ||</t>
   </si>
 </sst>
 </file>
@@ -678,10 +687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F48AB1A-0610-42A2-9EC7-30248C957360}">
-  <dimension ref="B3:F47"/>
+  <dimension ref="B3:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -704,7 +713,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>2</v>
@@ -724,7 +733,7 @@
         <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
@@ -738,7 +747,7 @@
         <v>4</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
@@ -752,7 +761,7 @@
         <v>5</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
@@ -766,7 +775,7 @@
         <v>6</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
@@ -774,13 +783,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
@@ -794,7 +803,7 @@
         <v>8</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
@@ -808,7 +817,7 @@
         <v>9</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
@@ -816,7 +825,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>64</v>
@@ -830,7 +839,7 @@
         <v>64</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>39</v>
@@ -850,7 +859,7 @@
         <v>16</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
@@ -878,7 +887,7 @@
         <v>17</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
@@ -900,7 +909,7 @@
         <v>65</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>19</v>
@@ -928,13 +937,13 @@
         <v>20</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
@@ -948,7 +957,7 @@
         <v>21</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
@@ -976,7 +985,7 @@
         <v>23</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
@@ -990,7 +999,7 @@
         <v>11</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.3">
@@ -1004,7 +1013,7 @@
         <v>24</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.3">
@@ -1018,7 +1027,7 @@
         <v>25</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.3">
@@ -1032,7 +1041,7 @@
         <v>13</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.3">
@@ -1060,7 +1069,7 @@
         <v>27</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.3">
@@ -1068,7 +1077,7 @@
         <v>27</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>28</v>
@@ -1082,230 +1091,244 @@
         <v>28</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>29</v>
+        <v>84</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B32" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="F32" s="2" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B33" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="F33" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B34" s="2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B35" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="F35" s="2" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B36" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="F36" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="F37" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B38" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="F38" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B39" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="F39" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B40" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="F40" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B41" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="F41" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B42" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="F42" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B43" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C43" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>60</v>
+      <c r="F43" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B44" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>72</v>
+      <c r="F44" s="3" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B45" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="F45" s="2" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B46" s="2" t="s">
-        <v>67</v>
+        <v>15</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>51</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B47" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="F47" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B48" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se agrego el analizador sintactico, se empiezo a agregar los metodos para generar el arbol
</commit_message>
<xml_diff>
--- a/Calculo de primeros y siguientes.xlsx
+++ b/Calculo de primeros y siguientes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Camran1234\source\repos\Proyecto2_Lenguajes_Analizador_Sintactico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AD8087-CB4D-443D-9C54-24711FBFDBA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8AF43CA-63A3-46A1-9891-B9A0A66854D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{02987567-9D64-471F-979D-34ECD3E91EEB}"/>
+    <workbookView xWindow="-8580" yWindow="5052" windowWidth="17280" windowHeight="8964" xr2:uid="{02987567-9D64-471F-979D-34ECD3E91EEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Primeros" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="93">
   <si>
     <t>Calculo de primeros</t>
   </si>
@@ -261,9 +261,6 @@
     <t>Primeros</t>
   </si>
   <si>
-    <t>Entero, Cadena, Chart, Decimal, Boolean</t>
-  </si>
-  <si>
     <t>"," , e</t>
   </si>
   <si>
@@ -289,6 +286,24 @@
   </si>
   <si>
     <t>= , " , " , ; , +, ), &amp;&amp;, ||</t>
+  </si>
+  <si>
+    <t>Entero, Cadena, Chart, Decimal, Boolean, Variable</t>
+  </si>
+  <si>
+    <t>Entero, Cadena, Chart, Decimal, Boolean,  Variable</t>
+  </si>
+  <si>
+    <t>Entero, Cadena, Chart, Decimal, Boolean, }, SI, MIENTRAS, HACER, DESDE, Variable IMPRIMIR, Leer</t>
+  </si>
+  <si>
+    <t>Fe</t>
+  </si>
+  <si>
+    <t>++, --, =</t>
+  </si>
+  <si>
+    <t>Entero, Cadena, Chart, Decimal, Boolean, }, SI, MIENTRAS, HACER, DESDE,Variable, IMPRIMIR, Leer</t>
   </si>
 </sst>
 </file>
@@ -312,7 +327,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -328,6 +343,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -359,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -371,6 +392,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -687,9 +714,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F48AB1A-0610-42A2-9EC7-30248C957360}">
-  <dimension ref="B3:F48"/>
+  <dimension ref="B3:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C9" workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
@@ -782,8 +809,8 @@
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>71</v>
+      <c r="C9" s="5" t="s">
+        <v>89</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>7</v>
@@ -824,8 +851,8 @@
       <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>78</v>
+      <c r="C12" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>64</v>
@@ -838,81 +865,81 @@
       <c r="B13" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>78</v>
+      <c r="C13" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>39</v>
+        <v>90</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>87</v>
+      <c r="F14" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>54</v>
+      <c r="F15" s="3" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="F16" s="2" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="F17" s="2" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>54</v>
@@ -920,13 +947,13 @@
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>54</v>
@@ -934,27 +961,27 @@
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="F20" s="2" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>71</v>
@@ -962,83 +989,83 @@
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="F22" s="2" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="F23" s="2" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="F24" s="2" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="F25" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>47</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>71</v>
@@ -1046,139 +1073,139 @@
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B28" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="F28" s="2" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B29" s="2" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>49</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B30" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="F30" s="2" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B31" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>84</v>
-      </c>
       <c r="F31" s="2" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B32" s="2" t="s">
-        <v>84</v>
+        <v>28</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>85</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>29</v>
+        <v>83</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B33" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="F33" s="2" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B34" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="F34" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B35" s="2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B36" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="F36" s="2" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B37" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>71</v>
@@ -1186,13 +1213,13 @@
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B38" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>71</v>
@@ -1200,13 +1227,13 @@
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B39" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>71</v>
@@ -1214,13 +1241,13 @@
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B40" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>71</v>
@@ -1228,13 +1255,13 @@
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B41" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>71</v>
@@ -1242,13 +1269,13 @@
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B42" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>71</v>
@@ -1256,13 +1283,13 @@
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B43" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>71</v>
@@ -1270,65 +1297,79 @@
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B44" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C44" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>60</v>
+      <c r="F44" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B45" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>71</v>
+      <c r="F45" s="3" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B46" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="F46" s="2" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B47" s="2" t="s">
-        <v>67</v>
+        <v>15</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>51</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B48" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="F48" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B49" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>